<commit_message>
last update for today
</commit_message>
<xml_diff>
--- a/BioPages/BrotherBios/Member Bios.xlsx
+++ b/BioPages/BrotherBios/Member Bios.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19560" windowHeight="8355"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="8355"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t xml:space="preserve">Name </t>
   </si>
@@ -134,40 +134,55 @@
 I also grew up in the suburbs of New Orleans.</t>
   </si>
   <si>
-    <t>Kierna Mason(no photo)</t>
-  </si>
-  <si>
     <t>My name is Chandler Key. I am a sophomore Mechanical Engineering Major and I plan to graduate sometime in 2017.</t>
   </si>
   <si>
     <t xml:space="preserve"> I like to play basketball and I have an identical twin sister.</t>
   </si>
   <si>
-    <t>Scott Stanford(no photo)X</t>
-  </si>
-  <si>
-    <t>Adrianne Duncan(no photo)X</t>
-  </si>
-  <si>
-    <t>Jasmine RobinsonX</t>
-  </si>
-  <si>
-    <t>Habeeb Kotun Jr(no photo)X</t>
-  </si>
-  <si>
-    <t>Derek Smith(no photo)X</t>
-  </si>
-  <si>
-    <t>Anthony AddingtonX(no photo)</t>
-  </si>
-  <si>
-    <t>Chandler Key(no photo)X</t>
-  </si>
-  <si>
-    <t>Alisa Howell(done)</t>
-  </si>
-  <si>
-    <t>Jimmy L. Scales Jr.(done)</t>
+    <t>Kierna Mason</t>
+  </si>
+  <si>
+    <t>Scott Stanford</t>
+  </si>
+  <si>
+    <t>Adrianne Duncan</t>
+  </si>
+  <si>
+    <t>Jimmy L. Scales Jr.</t>
+  </si>
+  <si>
+    <t>Jasmine Robinson</t>
+  </si>
+  <si>
+    <t>Habeeb Kotun Jr</t>
+  </si>
+  <si>
+    <t>Charles Rogers(need bio)</t>
+  </si>
+  <si>
+    <t>Chandler Key(no photo)</t>
+  </si>
+  <si>
+    <t>Alisa Howell</t>
+  </si>
+  <si>
+    <t>Anthony Addington(no photo)</t>
+  </si>
+  <si>
+    <t>Derek Smith(no photo)</t>
+  </si>
+  <si>
+    <t>Alise Waters(missing all)</t>
+  </si>
+  <si>
+    <t>Anothony Ellis(missing all)</t>
+  </si>
+  <si>
+    <t>Kenneth Njugunda(missing all)</t>
+  </si>
+  <si>
+    <t>Shabir Bhegandi(missing all)</t>
   </si>
 </sst>
 </file>
@@ -537,7 +552,7 @@
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -560,7 +575,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
@@ -615,7 +630,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>15</v>
@@ -626,7 +641,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>17</v>
@@ -637,7 +652,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>19</v>
@@ -670,7 +685,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>27</v>
@@ -681,7 +696,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>29</v>
@@ -706,61 +721,76 @@
         <v>42</v>
       </c>
       <c r="B15" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="12" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="B16" s="6"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
+        <v>46</v>
+      </c>
       <c r="B17" s="6"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="10" t="s">
+        <v>47</v>
+      </c>
       <c r="B18" s="6"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="10" t="s">
+        <v>48</v>
+      </c>
       <c r="B19" s="6"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="10" t="s">
+        <v>49</v>
+      </c>
       <c r="B20" s="6"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B21" s="6"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B22" s="6"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B23" s="6"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B24" s="6"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B25" s="6"/>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B26" s="6"/>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B27" s="6"/>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B28" s="6"/>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B29" s="6"/>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B30" s="6"/>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B31" s="6"/>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B32" s="6"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.2">

</xml_diff>